<commit_message>
update - Mar 21
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clegge\OneDrive - Wellcome Cloud\GitHub - R Projects\IATI_research_and_innovation\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clegge\OneDrive - Wellcome Cloud\GitHub - R Projects\ODA_research_and_innovation\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="102_{9C443570-9D5E-4CD5-A4D9-AFAFE3A24CAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="102_{9C443570-9D5E-4CD5-A4D9-AFAFE3A24CAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{CF93D44E-3BBB-4411-B445-C5E8AF06BDEA}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1188" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$D$941</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$939</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,32 +33,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
+  <si>
+    <t>iati_id</t>
+  </si>
+  <si>
+    <t>gov_funder</t>
+  </si>
+  <si>
+    <t>funding_iati_id</t>
+  </si>
+  <si>
+    <t>fund</t>
+  </si>
   <si>
     <t>extending_org</t>
   </si>
   <si>
-    <t>FCDO</t>
-  </si>
-  <si>
     <t>GB-COH-RC000797-GB-GOV-1-300484-RIAH</t>
   </si>
   <si>
+    <t>Foreign, Commonwealth and Development Office</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300484</t>
+  </si>
+  <si>
     <t>University of Manchester</t>
   </si>
   <si>
-    <t>iati_id</t>
-  </si>
-  <si>
-    <t>gov_funder</t>
-  </si>
-  <si>
-    <t>fund</t>
-  </si>
-  <si>
     <t>DAC-1601-OPP1182425</t>
   </si>
   <si>
+    <t>GB-GOV-1-300442</t>
+  </si>
+  <si>
     <t>Bill &amp; Melinda Gates Foundation</t>
   </si>
   <si>
@@ -77,46 +86,112 @@
     <t>DAC-1601-OPP1215722</t>
   </si>
   <si>
+    <t>DAC-1601-OPP1182843</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300126</t>
+  </si>
+  <si>
+    <t>IDRC</t>
+  </si>
+  <si>
+    <t>GB-COH-05543952-GB-1-203048</t>
+  </si>
+  <si>
+    <t>GB-1-203048</t>
+  </si>
+  <si>
+    <t>Cardno Emerging Markets</t>
+  </si>
+  <si>
+    <t>GB-COH-06274284-TEA2</t>
+  </si>
+  <si>
+    <t>GB-1-204867</t>
+  </si>
+  <si>
+    <t>Carbon Trust Advisory Ltd</t>
+  </si>
+  <si>
+    <t>GB-COH-03580586-SPHEIR</t>
+  </si>
+  <si>
+    <t>GB-1-203166</t>
+  </si>
+  <si>
+    <t>British Council</t>
+  </si>
+  <si>
+    <t>XM-DAC-47015-18199_BILATERAL_UNITEDKINGDOM-DFID-DEPARTMENTFORINTERNATIONALDEVELOPMENT_ILRI</t>
+  </si>
+  <si>
+    <t>CGIAR</t>
+  </si>
+  <si>
+    <t>GB-CHC-287287-DFID-PEDL</t>
+  </si>
+  <si>
+    <t>GB-1-202835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre for Economic Policy Research </t>
+  </si>
+  <si>
     <t>XM-DAC-301-2-109204-001</t>
   </si>
   <si>
-    <t>IDRC</t>
-  </si>
-  <si>
     <t>XM-DAC-301-2-109220-002</t>
   </si>
   <si>
     <t>XM-DAC-301-2-109238-002</t>
   </si>
   <si>
-    <t>300484: BEPAC - Building an evidence base on the protection of people affected by conflict</t>
-  </si>
-  <si>
-    <t>300442: GRID3 - Geo-Referenced Infrastructure and Demographic Data for Development</t>
-  </si>
-  <si>
-    <t>300126: CLARE - CLimate And REsilience Framework Programme Transition Phase</t>
-  </si>
-  <si>
-    <t>DAC-1601-OPP1182843</t>
-  </si>
-  <si>
-    <t>GB-COH-05543952-GB-1-203048</t>
-  </si>
-  <si>
-    <t>203048: Improved Rural Roads and Transport Services for Communities in Low Income Countries</t>
-  </si>
-  <si>
-    <t>Cardno Emerging Markets</t>
-  </si>
-  <si>
-    <t>204867: TEA - Transforming Energy Access</t>
-  </si>
-  <si>
-    <t>Carbon Trust Advisory Ltd</t>
-  </si>
-  <si>
-    <t>GB-COH-06274284-TEA2</t>
+    <t>GB-CHC-228248-R0500</t>
+  </si>
+  <si>
+    <t>GB-1-201009</t>
+  </si>
+  <si>
+    <t>FCDO Research &amp; Evidence Division</t>
+  </si>
+  <si>
+    <t>GB-CHC-228248-GAGE</t>
+  </si>
+  <si>
+    <t>GB-1-203529</t>
+  </si>
+  <si>
+    <t>GB-COH-02394229-UKACE</t>
+  </si>
+  <si>
+    <t>GB-1-203752</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	US-EIN-33-1112770-DFID_192010_LEIA_Business_Case</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	GB-CHC-228248-F0192300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	GB-GOV-1-300288</t>
+  </si>
+  <si>
+    <t>US-EIN-58-2368165-GB-GOV-1-300403</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300403</t>
+  </si>
+  <si>
+    <t>US-EIN-58-2368165-US-EIN-58-2368165-GB-GOV-1-203448</t>
+  </si>
+  <si>
+    <t>XM-DAC-47021-1394-DFID</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300649</t>
   </si>
 </sst>
 </file>
@@ -179,7 +254,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -190,6 +276,452 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD4F6C7F-8FFE-4C17-9CD7-266CCA4DB567}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3253740" y="4381500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="AutoShape 2" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A10705F-405B-4E1E-9EF1-513FB0136091}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8511540" y="4381500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F6F66E8-CB39-4C39-85E9-FF64998A6AFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10828020" y="4381500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="AutoShape 4" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F41D3B89-59C0-48B8-B0D8-EC8840AF2385}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3253740" y="4564380"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1029" name="AutoShape 5" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA610586-C7DB-4FE3-AC82-B7E29B972DD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8511540" y="4564380"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1030" name="AutoShape 6" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8F321EB-B3D8-4388-9B20-620E7FD9C614}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10828020" y="4564380"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132503</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1031" name="AutoShape 7" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBAA1563-90E3-4C6A-8A3E-4B3CBBC68711}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3253740" y="4747260"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132503</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1032" name="AutoShape 8" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BD42231-9595-4DC1-9267-EC9D56C97936}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8511540" y="4747260"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>132503</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1033" name="AutoShape 9" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18EF90D8-B7F7-4592-AC73-BAFD30AC70D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10828020" y="4747260"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -492,187 +1024,393 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.796875" customWidth="1"/>
-    <col min="2" max="2" width="15.09765625" customWidth="1"/>
-    <col min="3" max="3" width="52.19921875" customWidth="1"/>
-    <col min="4" max="4" width="37.19921875" customWidth="1"/>
+    <col min="1" max="1" width="42.69921875" customWidth="1"/>
+    <col min="2" max="2" width="42.09765625" customWidth="1"/>
+    <col min="3" max="3" width="26.8984375" customWidth="1"/>
+    <col min="4" max="4" width="30.3984375" customWidth="1"/>
+    <col min="5" max="5" width="37.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
@@ -710,21 +1448,23 @@
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="2"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D941" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}"/>
+  <autoFilter ref="A1:E939" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
+    <sortState ref="A2:E99">
+      <sortCondition ref="A1:A939"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="http://d-portal.org/q.html?aid=DAC-1601-OPP1195002" xr:uid="{935892AB-816C-451B-A6B2-D3FB021642A0}"/>
-    <hyperlink ref="A8" r:id="rId2" display="http://d-portal.org/q.html?aid=DAC-1601-OPP1182843" xr:uid="{05DF69EB-10D9-4331-95D9-F05359DFA4E9}"/>
+    <hyperlink ref="A7" r:id="rId1" display="http://d-portal.org/q.html?aid=DAC-1601-OPP1195002" xr:uid="{935892AB-816C-451B-A6B2-D3FB021642A0}"/>
+    <hyperlink ref="A6" r:id="rId2" display="http://d-portal.org/q.html?aid=DAC-1601-OPP1182843" xr:uid="{05DF69EB-10D9-4331-95D9-F05359DFA4E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -963,21 +1703,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1001,27 +1741,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9e449739-2858-4f41-8e5c-7dc6df20853e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="05c15269-663a-4da2-bb2b-1510839404b9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="05c15269-663a-4da2-bb2b-1510839404b9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9e449739-2858-4f41-8e5c-7dc6df20853e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update - May 21
Tidying of partner activity scripts and gov funder labels
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clegge\OneDrive - Wellcome Cloud\GitHub - R Projects\ODA_research_and_innovation\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="102_{9C443570-9D5E-4CD5-A4D9-AFAFE3A24CAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{CF93D44E-3BBB-4411-B445-C5E8AF06BDEA}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="102_{9C443570-9D5E-4CD5-A4D9-AFAFE3A24CAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1FE5017-3439-4EBD-8454-E9E1A7AA3E50}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1188" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$939</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$927</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>iati_id</t>
   </si>
@@ -50,123 +50,75 @@
     <t>extending_org</t>
   </si>
   <si>
+    <t>Foreign, Commonwealth and Development Office</t>
+  </si>
+  <si>
+    <t>FCDO Research &amp; Innovation</t>
+  </si>
+  <si>
+    <t>GB-CHC-287287-DFID-PEDL</t>
+  </si>
+  <si>
+    <t>GB-1-202835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre for Economic Policy Research </t>
+  </si>
+  <si>
+    <t>GB-CHC-228248-R0500</t>
+  </si>
+  <si>
+    <t>GB-1-201009</t>
+  </si>
+  <si>
+    <t>GB-CHC-228248-GAGE</t>
+  </si>
+  <si>
+    <t>GB-1-203529</t>
+  </si>
+  <si>
+    <t>GB-COH-03580586-SPHEIR</t>
+  </si>
+  <si>
+    <t>GB-1-203166</t>
+  </si>
+  <si>
+    <t>British Council</t>
+  </si>
+  <si>
+    <t>GB-COH-02394229-UKACE</t>
+  </si>
+  <si>
+    <t>GB-1-203752</t>
+  </si>
+  <si>
+    <t>GB-COH-05543952-GB-1-203048</t>
+  </si>
+  <si>
+    <t>GB-1-203048</t>
+  </si>
+  <si>
+    <t>Cardno Emerging Markets</t>
+  </si>
+  <si>
+    <t>GB-COH-06274284-TEA2</t>
+  </si>
+  <si>
+    <t>GB-1-204867</t>
+  </si>
+  <si>
+    <t>Carbon Trust Advisory Ltd</t>
+  </si>
+  <si>
     <t>GB-COH-RC000797-GB-GOV-1-300484-RIAH</t>
   </si>
   <si>
-    <t>Foreign, Commonwealth and Development Office</t>
-  </si>
-  <si>
     <t>GB-GOV-1-300484</t>
   </si>
   <si>
     <t>University of Manchester</t>
   </si>
   <si>
-    <t>DAC-1601-OPP1182425</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300442</t>
-  </si>
-  <si>
-    <t>Bill &amp; Melinda Gates Foundation</t>
-  </si>
-  <si>
-    <t>XI-IATI-CABI-DR10141</t>
-  </si>
-  <si>
-    <t>CABI</t>
-  </si>
-  <si>
-    <t>XI-IATI-CABI-AOI</t>
-  </si>
-  <si>
-    <t>DAC-1601-OPP1195002</t>
-  </si>
-  <si>
-    <t>DAC-1601-OPP1215722</t>
-  </si>
-  <si>
-    <t>DAC-1601-OPP1182843</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300126</t>
-  </si>
-  <si>
-    <t>IDRC</t>
-  </si>
-  <si>
-    <t>GB-COH-05543952-GB-1-203048</t>
-  </si>
-  <si>
-    <t>GB-1-203048</t>
-  </si>
-  <si>
-    <t>Cardno Emerging Markets</t>
-  </si>
-  <si>
-    <t>GB-COH-06274284-TEA2</t>
-  </si>
-  <si>
-    <t>GB-1-204867</t>
-  </si>
-  <si>
-    <t>Carbon Trust Advisory Ltd</t>
-  </si>
-  <si>
-    <t>GB-COH-03580586-SPHEIR</t>
-  </si>
-  <si>
-    <t>GB-1-203166</t>
-  </si>
-  <si>
-    <t>British Council</t>
-  </si>
-  <si>
-    <t>XM-DAC-47015-18199_BILATERAL_UNITEDKINGDOM-DFID-DEPARTMENTFORINTERNATIONALDEVELOPMENT_ILRI</t>
-  </si>
-  <si>
-    <t>CGIAR</t>
-  </si>
-  <si>
-    <t>GB-CHC-287287-DFID-PEDL</t>
-  </si>
-  <si>
-    <t>GB-1-202835</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centre for Economic Policy Research </t>
-  </si>
-  <si>
-    <t>XM-DAC-301-2-109204-001</t>
-  </si>
-  <si>
-    <t>XM-DAC-301-2-109220-002</t>
-  </si>
-  <si>
-    <t>XM-DAC-301-2-109238-002</t>
-  </si>
-  <si>
-    <t>GB-CHC-228248-R0500</t>
-  </si>
-  <si>
-    <t>GB-1-201009</t>
-  </si>
-  <si>
-    <t>FCDO Research &amp; Evidence Division</t>
-  </si>
-  <si>
-    <t>GB-CHC-228248-GAGE</t>
-  </si>
-  <si>
-    <t>GB-1-203529</t>
-  </si>
-  <si>
-    <t>GB-COH-02394229-UKACE</t>
-  </si>
-  <si>
-    <t>GB-1-203752</t>
-  </si>
-  <si>
     <t xml:space="preserve">	US-EIN-33-1112770-DFID_192010_LEIA_Business_Case</t>
   </si>
   <si>
@@ -192,6 +144,63 @@
   </si>
   <si>
     <t>GB-GOV-1-300649</t>
+  </si>
+  <si>
+    <t>ZA-NPO-048-364-FCFA_AG_CCKE</t>
+  </si>
+  <si>
+    <t>GB-1-203835</t>
+  </si>
+  <si>
+    <t>SouthSouthNorth</t>
+  </si>
+  <si>
+    <t>ZA-NPO-048-364-FCFA_AG_ADAPTATIONRESEARCHALLIANCE</t>
+  </si>
+  <si>
+    <t>ZA-NPO-048-364-FCFA_AG_ClimateMainstreamingFacility</t>
+  </si>
+  <si>
+    <t>ZA-NPO-048-364-FCFA_AG_ModelEvaluationHub/LaunchPad</t>
+  </si>
+  <si>
+    <t>ZA-NPO-048-364-FCFA_AG_Programme</t>
+  </si>
+  <si>
+    <t>GB-COH-877338-PP15011</t>
+  </si>
+  <si>
+    <t>GB-1-204427</t>
+  </si>
+  <si>
+    <t>Institute of Development Studies</t>
+  </si>
+  <si>
+    <t>CA-CRA_ACR-811793611-HGC</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300574</t>
+  </si>
+  <si>
+    <t>Grand Challenges Canada</t>
+  </si>
+  <si>
+    <t>US-EIN-04-2103547-VAXCYTE (FMR SUTROVAX)</t>
+  </si>
+  <si>
+    <t>Boston University</t>
+  </si>
+  <si>
+    <t>Department of Health and Social Care</t>
+  </si>
+  <si>
+    <t>US-EIN-04-2103547-INTEGRATED BIOTHERAPEUTICS</t>
+  </si>
+  <si>
+    <t>GB-GOV-10-GAMRIF-WP2-CARB-X</t>
+  </si>
+  <si>
+    <t>Global Health Security - GAMRIF</t>
   </si>
 </sst>
 </file>
@@ -254,7 +263,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -284,14 +313,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>132504</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>130599</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -333,14 +362,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>132504</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>130599</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -382,14 +411,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>132504</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>130599</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -431,14 +460,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>132504</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>130599</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -480,14 +509,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>132504</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>130599</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -529,14 +558,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>132504</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>130599</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -576,35 +605,136 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>130598</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1032" name="AutoShape 8" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BD42231-9595-4DC1-9267-EC9D56C97936}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8511540" y="4747260"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>130598</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1033" name="AutoShape 9" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18EF90D8-B7F7-4592-AC73-BAFD30AC70D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10828020" y="4747260"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>132503</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132505</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1031" name="AutoShape 7" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBAA1563-90E3-4C6A-8A3E-4B3CBBC68711}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3253740" y="4747260"/>
-          <a:ext cx="304800" cy="304800"/>
+        <xdr:cNvPr id="11" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23B1E10F-08D1-4442-BF1A-6902BE8269BC}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{18EF90D8-B7F7-4592-AC73-BAFD30AC70D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3257550" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -625,35 +755,90 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132505</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 4" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA32B180-C7AF-48B8-827F-623237F5D682}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{23B1E10F-08D1-4442-BF1A-6902BE8269BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3257550" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>132503</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132505</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1032" name="AutoShape 8" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BD42231-9595-4DC1-9267-EC9D56C97936}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8511540" y="4747260"/>
-          <a:ext cx="304800" cy="304800"/>
+        <xdr:cNvPr id="14" name="AutoShape 2" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{855D1109-5DF9-4024-8031-723554D2BDAF}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{1B57B9B7-1215-4AE4-A1F1-C58C9FABB570}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8515350" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -674,35 +859,766 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132505</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 5" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FE6E078-594C-44A1-ABAA-A9EFDCB20C55}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{855D1109-5DF9-4024-8031-723554D2BDAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8515350" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 8" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05EEA077-04B8-44EF-BDC1-DFB2157AF681}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4FE6E078-594C-44A1-ABAA-A9EFDCB20C55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8515350" y="2571750"/>
+          <a:ext cx="304800" cy="307763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>132503</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1033" name="AutoShape 9" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+        <xdr:cNvPr id="17" name="AutoShape 3" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C289A2E-0147-4157-9A2D-62F7446CD72D}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{05EEA077-04B8-44EF-BDC1-DFB2157AF681}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>132503</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 6" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86D786F6-0527-4A38-9ADD-44DCD9541EF1}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{1C289A2E-0147-4157-9A2D-62F7446CD72D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>132502</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="AutoShape 9" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7983B2AA-F910-4D7A-9B7F-FB6B7D807E6A}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{86D786F6-0527-4A38-9ADD-44DCD9541EF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2571750"/>
+          <a:ext cx="304800" cy="307763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130598</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A63B77D-3762-4952-9317-B6D80E22B15C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7983B2AA-F910-4D7A-9B7F-FB6B7D807E6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3257550" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130598</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="AutoShape 2" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDCB1EBA-0CD2-411D-BCB2-CA0037EA59E2}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{0A63B77D-3762-4952-9317-B6D80E22B15C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8515350" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130598</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="AutoShape 3" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE6A2B49-AEB1-4EFF-9E01-00AE44155411}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DDCB1EBA-0CD2-411D-BCB2-CA0037EA59E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130598</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="AutoShape 5" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B3B37DF-2C74-49CC-85FA-97F9DC6A8D8B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{915D4764-B360-4B34-A1C4-EA17BDC9338B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8515350" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130598</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="AutoShape 6" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B858B64-3181-4777-A71F-01C8247C4AAE}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{1B3B37DF-2C74-49CC-85FA-97F9DC6A8D8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130597</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="AutoShape 8" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51E7F655-36DE-4420-8BB3-7923EC94C2FD}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{80F39D52-8432-4ACD-AE27-0CDB386C596A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8515350" y="2571750"/>
+          <a:ext cx="304800" cy="307763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130597</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="AutoShape 9" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3631F096-B2C7-45BC-9D50-8108E99AF4F0}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{51E7F655-36DE-4420-8BB3-7923EC94C2FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2571750"/>
+          <a:ext cx="304800" cy="307763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6343758F-4837-4A09-A307-1B9C983F314C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{3631F096-B2C7-45BC-9D50-8108E99AF4F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3257550" y="2752725"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="AutoShape 4" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56AE0943-A4B1-4CDD-9735-21BFEC8F07D3}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{6343758F-4837-4A09-A307-1B9C983F314C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3257550" y="2752725"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>132503</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="AutoShape 7" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18EF90D8-B7F7-4592-AC73-BAFD30AC70D9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10828020" y="4747260"/>
-          <a:ext cx="304800" cy="304800"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5FA85D6-C8D8-4CF6-9B37-703E261C692C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{56AE0943-A4B1-4CDD-9735-21BFEC8F07D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3257550" y="2752725"/>
+          <a:ext cx="304800" cy="307763"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -721,6 +1637,1684 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="AutoShape 2" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E53E9F78-E6E7-4904-B328-CA99608AC29C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F5FA85D6-C8D8-4CF6-9B37-703E261C692C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8515350" y="2752725"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="AutoShape 5" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F351A2F2-33E7-4A50-B944-CCA58A0A94CF}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E53E9F78-E6E7-4904-B328-CA99608AC29C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8515350" y="2752725"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132505</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="AutoShape 3" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9EB713E-A7E1-4E39-BC3C-724AE42A8225}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{BC7FE2B8-3764-46D4-A626-7620381EF52E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2400300"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132505</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="AutoShape 6" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C62959F7-F978-4A50-8610-43427E99BE2B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C9EB713E-A7E1-4E39-BC3C-724AE42A8225}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2400300"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="AutoShape 9" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6159DD88-3DB8-40F2-B2E0-AA5E72192954}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C62959F7-F978-4A50-8610-43427E99BE2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2400300"/>
+          <a:ext cx="304800" cy="307763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="AutoShape 3" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5C93B1B-C6FC-4892-8921-81253B057D36}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{413A65FA-201E-48CA-A8D0-5DE47E1D10C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>132504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="AutoShape 6" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC193773-728F-42E4-9F3D-2F24F52402A5}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{A716C405-D03F-4678-AC83-DE8D95CBA6B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2571750"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>132503</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="AutoShape 9" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14B298BB-CE12-4C96-BCA7-C096DEAC596F}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F4804472-2E12-4BDE-BE53-B0052769BD90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2571750"/>
+          <a:ext cx="304800" cy="307763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>130600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC05C223-E5EA-4EAB-B357-705F0BC8B7F5}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{14B298BB-CE12-4C96-BCA7-C096DEAC596F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3257550" y="2752725"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>130600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="AutoShape 4" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DD8A67F-D767-42B0-B954-92E0EE2704F7}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{EC05C223-E5EA-4EAB-B357-705F0BC8B7F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3257550" y="2752725"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130598</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="AutoShape 3" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A7EF032-7ADB-4754-9D61-CC0B964125AC}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{8CB30E19-646A-49F0-A677-F32E3E7CF569}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2400300"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130598</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="AutoShape 6" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B665B7DA-3F6C-4007-9CA9-B281DF9FA237}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4A7EF032-7ADB-4754-9D61-CC0B964125AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2400300"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>130597</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="AutoShape 9" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE8E5113-92C5-481A-884D-D21462B91B22}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B665B7DA-3F6C-4007-9CA9-B281DF9FA237}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2400300"/>
+          <a:ext cx="304800" cy="307763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>130600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="AutoShape 3" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86360944-833A-4E68-A572-C0009A99E678}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{EE8E5113-92C5-481A-884D-D21462B91B22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2752725"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>130600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="AutoShape 6" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3820B6AE-5649-4ADB-B475-950CE7725342}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{86360944-833A-4E68-A572-C0009A99E678}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2752725"/>
+          <a:ext cx="304800" cy="307764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>130599</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="AutoShape 9" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3CC8D54-E49C-4EFD-872F-D755090FFC79}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{3820B6AE-5649-4ADB-B475-950CE7725342}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10829925" y="2752725"/>
+          <a:ext cx="304800" cy="307763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="299933"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9842338-5221-4260-B0ED-7D65677006A7}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{14B298BB-CE12-4C96-BCA7-C096DEAC596F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3217333"/>
+          <a:ext cx="304800" cy="299933"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="305647"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F13BBF7-EBBE-4C18-B1F6-0143516F175A}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{3631F096-B2C7-45BC-9D50-8108E99AF4F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3048000"/>
+          <a:ext cx="304800" cy="305647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="305647"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="AutoShape 4" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA200BA0-052C-4966-AF81-494A7631ECCC}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{6343758F-4837-4A09-A307-1B9C983F314C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3048000"/>
+          <a:ext cx="304800" cy="305647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="305646"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="AutoShape 7" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96B37F20-8AB6-48E2-B99D-41457A013A57}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{56AE0943-A4B1-4CDD-9735-21BFEC8F07D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3048000"/>
+          <a:ext cx="304800" cy="305646"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="303743"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="71" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E383E2A9-B8AD-4DB9-90B7-18D33E2CBF87}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{14B298BB-CE12-4C96-BCA7-C096DEAC596F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3217333"/>
+          <a:ext cx="304800" cy="303743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="303743"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="AutoShape 4" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EDFD31F-40A1-4EB6-B98D-585971E966D4}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{EC05C223-E5EA-4EAB-B357-705F0BC8B7F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3217333"/>
+          <a:ext cx="304800" cy="303743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="301837"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="AutoShape 2" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CF367B1-A9AA-4EEF-B195-894C20701044}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F5FA85D6-C8D8-4CF6-9B37-703E261C692C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8519583" y="3048000"/>
+          <a:ext cx="304800" cy="301837"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="301837"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="AutoShape 5" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F9CC930-5831-4308-A3E8-911785261CE7}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E53E9F78-E6E7-4904-B328-CA99608AC29C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8519583" y="3048000"/>
+          <a:ext cx="304800" cy="301837"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="299933"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D16127C-0D31-43D1-BA07-4BA1594B0B14}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{14B298BB-CE12-4C96-BCA7-C096DEAC596F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3217333"/>
+          <a:ext cx="304800" cy="299933"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="299933"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="AutoShape 4" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABE8B45F-5D9C-42C5-AC06-304AA4DD8601}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{EC05C223-E5EA-4EAB-B357-705F0BC8B7F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3217333"/>
+          <a:ext cx="304800" cy="299933"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="299933"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D8EF856-3C18-4916-8247-7DE254777DB3}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{14B298BB-CE12-4C96-BCA7-C096DEAC596F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3386667"/>
+          <a:ext cx="304800" cy="299933"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="305647"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{600FC9C0-BCD5-44E6-ABBC-1F58884A74BA}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{3631F096-B2C7-45BC-9D50-8108E99AF4F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3217333"/>
+          <a:ext cx="304800" cy="305647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="305647"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="AutoShape 4" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2D89069-5746-4430-954B-BEB9EF563034}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{6343758F-4837-4A09-A307-1B9C983F314C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3217333"/>
+          <a:ext cx="304800" cy="305647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="305646"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="AutoShape 7" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBE9C09A-447E-4948-8782-80A78E3AE163}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{56AE0943-A4B1-4CDD-9735-21BFEC8F07D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3217333"/>
+          <a:ext cx="304800" cy="305646"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="303743"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="AutoShape 1" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56550E7B-EE14-4092-98D7-8715AE9C5507}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{14B298BB-CE12-4C96-BCA7-C096DEAC596F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3386667"/>
+          <a:ext cx="304800" cy="303743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="303743"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="AutoShape 4" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F926930-9D7B-4E4C-BFE6-A508BEEA4AF9}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{EC05C223-E5EA-4EAB-B357-705F0BC8B7F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3259667" y="3386667"/>
+          <a:ext cx="304800" cy="303743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="301837"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="AutoShape 2" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8311357-343E-46C8-8A83-5B974DD1B680}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F5FA85D6-C8D8-4CF6-9B37-703E261C692C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8519583" y="3217333"/>
+          <a:ext cx="304800" cy="301837"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="301837"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="AutoShape 5" descr="http://127.0.0.1:11466/grid_resource/object-viewer.png">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15E9DD51-BC33-48C1-9538-326DA0F18916}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E53E9F78-E6E7-4904-B328-CA99608AC29C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8519583" y="3217333"/>
+          <a:ext cx="304800" cy="301837"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1024,16 +3618,16 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.69921875" customWidth="1"/>
+    <col min="1" max="1" width="54.69921875" customWidth="1"/>
     <col min="2" max="2" width="42.09765625" customWidth="1"/>
     <col min="3" max="3" width="26.8984375" customWidth="1"/>
     <col min="4" max="4" width="30.3984375" customWidth="1"/>
@@ -1059,70 +3653,64 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,210 +3718,219 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
         <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
         <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
         <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
         <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
         <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>39</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
+      <c r="A17" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>39</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>39</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>29</v>
+      <c r="A19" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>39</v>
-      </c>
-      <c r="E19" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1341,41 +3938,50 @@
         <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
         <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" t="s">
-        <v>39</v>
+      <c r="E21" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1383,28 +3989,53 @@
         <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" t="s">
-        <v>39</v>
-      </c>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
@@ -1412,55 +4043,25 @@
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="2"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="2"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="2"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="2"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E939" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
-    <sortState ref="A2:E99">
-      <sortCondition ref="A1:A939"/>
+  <autoFilter ref="A1:E927" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
+    <sortState ref="A2:E87">
+      <sortCondition ref="A1:A927"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="A20:A1048576 A1:A16 A18">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" display="http://d-portal.org/q.html?aid=DAC-1601-OPP1195002" xr:uid="{935892AB-816C-451B-A6B2-D3FB021642A0}"/>
-    <hyperlink ref="A6" r:id="rId2" display="http://d-portal.org/q.html?aid=DAC-1601-OPP1182843" xr:uid="{05DF69EB-10D9-4331-95D9-F05359DFA4E9}"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://d-portal.org/q.html?aid=DAC-1601-OPP1182843" xr:uid="{05DF69EB-10D9-4331-95D9-F05359DFA4E9}"/>
+    <hyperlink ref="A3" r:id="rId2" display="http://d-portal.org/q.html?aid=DAC-1601-OPP1195002" xr:uid="{935892AB-816C-451B-A6B2-D3FB021642A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1469,6 +4070,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6713CC7F31D7C498DF06765AF1263E4" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="49295815813be5682bd1502ac40ad112">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="9e449739-2858-4f41-8e5c-7dc6df20853e" xmlns:ns4="05c15269-663a-4da2-bb2b-1510839404b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57db594e689bb932d2839527134c19ea" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1702,25 +4321,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="05c15269-663a-4da2-bb2b-1510839404b9"/>
+    <ds:schemaRef ds:uri="9e449739-2858-4f41-8e5c-7dc6df20853e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E21D5880-A9EF-4322-906E-79CE5A8FFAC1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1738,30 +4365,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9e449739-2858-4f41-8e5c-7dc6df20853e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="05c15269-663a-4da2-bb2b-1510839404b9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Transaction extract added 20/7
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clegge\OneDrive - Wellcome Cloud\My Documents\GitHub\ODA_research_and_innovation\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dfid-my.sharepoint.com/personal/e-clegg_dfid_gov_uk/Documents/Github Projects/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="102_{9C443570-9D5E-4CD5-A4D9-AFAFE3A24CAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{F88995ED-5DE3-47D5-A3A7-CDB92950576A}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{CCECB9D9-E4EA-459C-8432-4D5A4B733364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{45F363C7-47C0-4147-B49F-9EF3E8721D19}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1188" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
   <sheets>
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$931</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$922</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -26,6 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="95">
   <si>
     <t>iati_id</t>
   </si>
@@ -50,33 +53,18 @@
     <t>extending_org</t>
   </si>
   <si>
-    <t>GB-CHC-287287-DFID-PEDL</t>
+    <t>GB-CHC-228248-R0500</t>
   </si>
   <si>
     <t>Foreign, Commonwealth and Development Office</t>
   </si>
   <si>
-    <t>GB-1-202835</t>
+    <t>GB-1-201009</t>
   </si>
   <si>
     <t>FCDO Research &amp; Innovation</t>
   </si>
   <si>
-    <t xml:space="preserve">Centre for Economic Policy Research </t>
-  </si>
-  <si>
-    <t>GB-CHC-228248-R0500</t>
-  </si>
-  <si>
-    <t>GB-1-201009</t>
-  </si>
-  <si>
-    <t>GB-CHC-228248-GAGE</t>
-  </si>
-  <si>
-    <t>GB-1-203529</t>
-  </si>
-  <si>
     <t>GB-COH-03580586-SPHEIR</t>
   </si>
   <si>
@@ -119,16 +107,16 @@
     <t>University of Manchester</t>
   </si>
   <si>
-    <t xml:space="preserve">	US-EIN-33-1112770-DFID_192010_LEIA_Business_Case</t>
+    <t>US-EIN-33-1112770-DFID_192010_LEIA_Business_Case</t>
   </si>
   <si>
     <t>GB-GOV-1-300111</t>
   </si>
   <si>
-    <t xml:space="preserve">	GB-CHC-228248-F0192300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	GB-GOV-1-300288</t>
+    <t>GB-CHC-228248-F0192300</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300288</t>
   </si>
   <si>
     <t>US-EIN-58-2368165-GB-GOV-1-300403</t>
@@ -167,130 +155,172 @@
     <t>ZA-NPO-048-364-FCFA_AG_Programme</t>
   </si>
   <si>
-    <t>GB-COH-877338-PP15011</t>
-  </si>
-  <si>
-    <t>GB-1-204427</t>
+    <t>CA-CRA_ACR-811793611-HGC</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300574</t>
+  </si>
+  <si>
+    <t>Grand Challenges Canada</t>
+  </si>
+  <si>
+    <t>GB-CHC-222655-PO6407</t>
+  </si>
+  <si>
+    <t>GB-1-203089</t>
+  </si>
+  <si>
+    <t>Liverpool School of Hygiene and Tropical Medicine</t>
+  </si>
+  <si>
+    <t>GB-CHC-222655-PO5247REBUILD</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-301133</t>
+  </si>
+  <si>
+    <t>GB-COH-RC000658 -NEWCLIMATEECONOMY</t>
+  </si>
+  <si>
+    <t>University of Leeds</t>
+  </si>
+  <si>
+    <t>GB-COH-RC000658 -GB-GOV-1-301132</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-301132</t>
+  </si>
+  <si>
+    <t>GB-EDU-133784-TWPCOP</t>
+  </si>
+  <si>
+    <t>University of Birmingham</t>
+  </si>
+  <si>
+    <t>GB-COH-RC000660-WAR-PATH</t>
+  </si>
+  <si>
+    <t>Department of Health and Social Care</t>
+  </si>
+  <si>
+    <t>Global Health Research - Programmes</t>
+  </si>
+  <si>
+    <t>University of Liverpool</t>
+  </si>
+  <si>
+    <t>DAC-1601-OPP1028264</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300728</t>
+  </si>
+  <si>
+    <t>Bill &amp; Melinda Gates Foundation</t>
+  </si>
+  <si>
+    <t>DAC-1601-OPP1052391</t>
+  </si>
+  <si>
+    <t>DAC-1601-OPPGD1394</t>
+  </si>
+  <si>
+    <t>DAC-1601-OPP1215722</t>
+  </si>
+  <si>
+    <t>DAC-1601-OPP1182425</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300442</t>
+  </si>
+  <si>
+    <t>DAC-1601-INV-018067</t>
+  </si>
+  <si>
+    <t>DAC-1601-INV-006162</t>
+  </si>
+  <si>
+    <t>GB-1-204773</t>
+  </si>
+  <si>
+    <t>GB-CHC-1177110-R2HC</t>
+  </si>
+  <si>
+    <t>Global Health Research - Partnerships</t>
+  </si>
+  <si>
+    <t>Elrha</t>
+  </si>
+  <si>
+    <t>FCDO partially funded</t>
+  </si>
+  <si>
+    <t>US-EIN-134166228-GB-GOV-1-300632-102</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300632</t>
+  </si>
+  <si>
+    <t>FCDO fully funded</t>
+  </si>
+  <si>
+    <t>Acumen</t>
+  </si>
+  <si>
+    <t>IN-MCA-U74140DL1998PLC097579-1662_AGRITECH-CATALYST_DFID_UK</t>
+  </si>
+  <si>
+    <t>GB-1-203067</t>
+  </si>
+  <si>
+    <t>IPE Global</t>
+  </si>
+  <si>
+    <t>CA-CRA_ACR-101182509-DFID-REGIONAL-SPARC</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300655</t>
+  </si>
+  <si>
+    <t>CowaterSogema International Inc</t>
+  </si>
+  <si>
+    <t>GB-COH-877338-RF15005</t>
+  </si>
+  <si>
+    <t>GB-1-204725</t>
   </si>
   <si>
     <t>Institute of Development Studies</t>
   </si>
   <si>
-    <t>CA-CRA_ACR-811793611-HGC</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300574</t>
-  </si>
-  <si>
-    <t>Grand Challenges Canada</t>
-  </si>
-  <si>
-    <t>Department of Health and Social Care</t>
-  </si>
-  <si>
-    <t>GB-GOV-10-GAMRIF-WP2-CARB-X</t>
-  </si>
-  <si>
-    <t>Global Health Security - GAMRIF</t>
-  </si>
-  <si>
-    <t>Boston University</t>
-  </si>
-  <si>
-    <t>GB-CHC-222655-PO6407</t>
-  </si>
-  <si>
-    <t>GB-1-203089</t>
-  </si>
-  <si>
-    <t>Liverpool School of Hygiene and Tropical Medicine</t>
-  </si>
-  <si>
-    <t>GB-CHC-222655-PO5247REBUILD</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-301133</t>
-  </si>
-  <si>
-    <t>University of Leeds</t>
-  </si>
-  <si>
-    <t>GB-EDU-133784-BACTIVAC-MR/R005974/1</t>
-  </si>
-  <si>
-    <t>University of Birmingham</t>
-  </si>
-  <si>
-    <t>Global Health Security - UK Vaccine Network</t>
-  </si>
-  <si>
-    <t>GB-EDU-133784-TWPCOP</t>
-  </si>
-  <si>
-    <t>GB-COH-RC000660-WAR-PATH</t>
-  </si>
-  <si>
-    <t>Global Health Research - Programmes</t>
-  </si>
-  <si>
-    <t>University of Liverpool</t>
-  </si>
-  <si>
-    <t>DAC-1601-OPP1052391</t>
-  </si>
-  <si>
-    <t>DAC-1601-OPPGD1394</t>
-  </si>
-  <si>
-    <t>DAC-1601-OPP1215722</t>
-  </si>
-  <si>
-    <t>Bill &amp; Melinda Gates Foundation</t>
-  </si>
-  <si>
-    <t>GB-GOV-10-GAMRIF-WP5-FIND</t>
-  </si>
-  <si>
-    <t>Foundation for New innovative Diagnostics</t>
-  </si>
-  <si>
-    <t>GB-GOV-10-GAMRIF-WP6-GARDP</t>
-  </si>
-  <si>
-    <t>Drugs for Neglected Diseases Initiative</t>
-  </si>
-  <si>
-    <t>US-EIN-04-2103547-LYTICA</t>
-  </si>
-  <si>
-    <t>US-EIN-04-2103547-BIOVERSYS</t>
-  </si>
-  <si>
-    <t>US-EIN-04-2103547-BB100</t>
-  </si>
-  <si>
-    <t>US-EIN-04-2103547-PROCARTA</t>
-  </si>
-  <si>
-    <t>US-EIN-04-2103547-VAXCYTE(FMRSUTROVAX)</t>
-  </si>
-  <si>
-    <t>US-EIN-04-2103547-INTEGRATEDBIOTHERAPEUTICS</t>
-  </si>
-  <si>
-    <t>GB-COH-RC000658-NEWCLIMATEECONOMY</t>
-  </si>
-  <si>
-    <t>GB-COH-877338-GV18012</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300211</t>
-  </si>
-  <si>
-    <t>GB-COH-877338-DI15009</t>
-  </si>
-  <si>
-    <t>GB-1-205121</t>
+    <t>GB-COH-03122495-A0534</t>
+  </si>
+  <si>
+    <t>Oxford Policy Management</t>
+  </si>
+  <si>
+    <t>GB-COH-03122495-A0014</t>
+  </si>
+  <si>
+    <t>GB-1-203051</t>
+  </si>
+  <si>
+    <t>US-EIN-134166228-GB-COH-06274284-TEA2 - PIONEER ENERGY INVESTMENT INITIATIVE 2</t>
+  </si>
+  <si>
+    <t>US-EIN-042103594-GCCI-3978870</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdul Latif Jameel Poverty Action Lab </t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300966</t>
+  </si>
+  <si>
+    <t>GB-GOV-10-R2HC</t>
   </si>
 </sst>
 </file>
@@ -353,7 +383,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -707,23 +747,23 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.69921875" customWidth="1"/>
-    <col min="2" max="2" width="42.09765625" customWidth="1"/>
-    <col min="3" max="3" width="31.69921875" customWidth="1"/>
-    <col min="4" max="4" width="30.3984375" customWidth="1"/>
-    <col min="5" max="5" width="37.19921875" customWidth="1"/>
+    <col min="1" max="1" width="54.75" customWidth="1"/>
+    <col min="2" max="2" width="42.08203125" customWidth="1"/>
+    <col min="3" max="3" width="31.75" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="37.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -740,7 +780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -753,25 +793,25 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -785,7 +825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -802,7 +842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -815,42 +855,42 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -863,55 +903,52 @@
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -922,8 +959,11 @@
       <c r="D13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -931,449 +971,480 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
         <v>41</v>
       </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>42</v>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>47</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
         <v>48</v>
       </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
         <v>54</v>
       </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D24" t="s">
         <v>55</v>
       </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="E24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>57</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
         <v>58</v>
       </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>60</v>
       </c>
-      <c r="B24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>62</v>
       </c>
-      <c r="E24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>63</v>
       </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
         <v>64</v>
       </c>
-      <c r="B26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="E26" t="s">
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>68</v>
       </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
         <v>73</v>
       </c>
-      <c r="B31" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D34" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="E34" t="s">
         <v>75</v>
       </c>
-      <c r="B32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>76</v>
       </c>
-      <c r="B33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
         <v>77</v>
       </c>
-      <c r="B34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" t="s">
         <v>78</v>
       </c>
-      <c r="B35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" t="s">
-        <v>52</v>
-      </c>
-      <c r="E35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="E39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="E40" t="s">
-        <v>46</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E922" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E82">
+      <sortCondition ref="A1:A922"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A16 A18 A20:A1048576">
+  <conditionalFormatting sqref="A34:A1048576 A16 A1:A14 A18:A21 A23:A32">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
+  <conditionalFormatting sqref="A33">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
+  <conditionalFormatting sqref="A22">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://d-portal.org/q.html?aid=DAC-1601-OPP1182843" xr:uid="{05DF69EB-10D9-4331-95D9-F05359DFA4E9}"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://d-portal.org/q.html?aid=DAC-1601-OPP1195002" xr:uid="{935892AB-816C-451B-A6B2-D3FB021642A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1381,6 +1452,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6713CC7F31D7C498DF06765AF1263E4" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="49295815813be5682bd1502ac40ad112">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="9e449739-2858-4f41-8e5c-7dc6df20853e" xmlns:ns4="05c15269-663a-4da2-bb2b-1510839404b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57db594e689bb932d2839527134c19ea" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1614,25 +1703,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E21D5880-A9EF-4322-906E-79CE5A8FFAC1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1650,30 +1739,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="05c15269-663a-4da2-bb2b-1510839404b9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e449739-2858-4f41-8e5c-7dc6df20853e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated after RI IATI tag added by FCDO
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dfid-my.sharepoint.com/personal/e-clegg_dfid_gov_uk/Documents/Github Projects/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{1F8182CB-FE63-4525-B953-FF5A791C5CBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9A00CC7-B8BF-4FB6-ACF9-584E0BF222D2}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{1F8182CB-FE63-4525-B953-FF5A791C5CBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA1F9899-4435-4D4B-B388-A993FEEDEA6B}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$908</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$898</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
   <si>
     <t>iati_id</t>
   </si>
@@ -77,30 +77,9 @@
     <t>GB-1-204867</t>
   </si>
   <si>
-    <t>GB-COH-RC000797-GB-GOV-1-300484-RIAH</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300484</t>
-  </si>
-  <si>
     <t>University of Manchester</t>
   </si>
   <si>
-    <t>US-EIN-33-1112770-DFID_192010_LEIA_Business_Case</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300111</t>
-  </si>
-  <si>
-    <t>GB-CHC-228248-F0192300</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300288</t>
-  </si>
-  <si>
-    <t>XM-DAC-47021-1394-DFID</t>
-  </si>
-  <si>
     <t>GB-GOV-1-300649</t>
   </si>
   <si>
@@ -134,21 +113,6 @@
     <t>Grand Challenges Canada</t>
   </si>
   <si>
-    <t>GB-CHC-222655-PO6407</t>
-  </si>
-  <si>
-    <t>GB-1-203089</t>
-  </si>
-  <si>
-    <t>Liverpool School of Hygiene and Tropical Medicine</t>
-  </si>
-  <si>
-    <t>GB-CHC-222655-PO5247REBUILD</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-301133</t>
-  </si>
-  <si>
     <t>GB-EDU-133784-TWPCOP</t>
   </si>
   <si>
@@ -197,15 +161,6 @@
     <t>DAC-1601-INV-006162</t>
   </si>
   <si>
-    <t>GB-CHC-1177110-R2HC</t>
-  </si>
-  <si>
-    <t>Global Health Research - Partnerships</t>
-  </si>
-  <si>
-    <t>Elrha</t>
-  </si>
-  <si>
     <t>US-EIN-134166228-GB-GOV-1-300632-102</t>
   </si>
   <si>
@@ -227,15 +182,6 @@
     <t>IPE Global</t>
   </si>
   <si>
-    <t>CA-CRA_ACR-101182509-DFID-REGIONAL-SPARC</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300655</t>
-  </si>
-  <si>
-    <t>CowaterSogema International Inc</t>
-  </si>
-  <si>
     <t>GB-COH-877338-RF15005</t>
   </si>
   <si>
@@ -257,15 +203,9 @@
     <t>US-EIN-134166228-GB-COH-06274284-TEA2 - PIONEER ENERGY INVESTMENT INITIATIVE 2</t>
   </si>
   <si>
-    <t>US-EIN-91-1157127-PATH CENTRE OF EXCELLENCE FOR MICROARRAY PATCH PLATFORM DEVELOPMENT (MAPS) (300341-112)</t>
-  </si>
-  <si>
     <t>US-EIN-91-1157127-RHSC_PROGRAM_2020-2025_(300713-103)</t>
   </si>
   <si>
-    <t>US-EIN-91-1157127-DAWN</t>
-  </si>
-  <si>
     <t>GB-GOV-1-300341</t>
   </si>
   <si>
@@ -291,6 +231,12 @@
   </si>
   <si>
     <t>IFPRI</t>
+  </si>
+  <si>
+    <t>GB-CHC-209131-A05500</t>
+  </si>
+  <si>
+    <t>GB-1-204043</t>
   </si>
 </sst>
 </file>
@@ -696,11 +642,11 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -740,7 +686,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -757,7 +703,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -765,47 +711,53 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -816,32 +768,35 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -850,7 +805,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -858,19 +813,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -878,84 +830,72 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -965,11 +905,14 @@
       <c r="B16" t="s">
         <v>5</v>
       </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -977,58 +920,67 @@
         <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
         <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1038,296 +990,149 @@
       <c r="B21" t="s">
         <v>5</v>
       </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" t="s">
-        <v>58</v>
-      </c>
-      <c r="E34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" t="s">
-        <v>58</v>
-      </c>
-      <c r="E37" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E908" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E68">
-      <sortCondition ref="A1:A908"/>
+  <autoFilter ref="A1:E898" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
+      <sortCondition ref="A1:A898"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A9">
+  <conditionalFormatting sqref="A5">
     <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
+  <conditionalFormatting sqref="A7">
     <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10 A1:A8 A12:A1048576">
+  <conditionalFormatting sqref="A6 A1:A4 A8:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update - Sep 21
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dfid-my.sharepoint.com/personal/e-clegg_dfid_gov_uk/Documents/Github Projects/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{1F8182CB-FE63-4525-B953-FF5A791C5CBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA1F9899-4435-4D4B-B388-A993FEEDEA6B}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{1F8182CB-FE63-4525-B953-FF5A791C5CBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{154CDFCA-834D-4DD5-94FD-EE2B301E65AB}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
+    <workbookView xWindow="-25320" yWindow="420" windowWidth="25440" windowHeight="15390" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
   <sheets>
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="76">
   <si>
     <t>iati_id</t>
   </si>
@@ -237,6 +237,33 @@
   </si>
   <si>
     <t>GB-1-204043</t>
+  </si>
+  <si>
+    <t>US-EIN-20-8530747-RESEARCH INITIATIVE EXPLORING THE USE OF EDTECH IN AFR/SAR</t>
+  </si>
+  <si>
+    <t>GB-1-205288</t>
+  </si>
+  <si>
+    <t>Results for Development</t>
+  </si>
+  <si>
+    <t>GB-COH-10333897-(SMEP) PROGRAMME – PROGRAMME MANAGEMENT COMPONENT</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300124</t>
+  </si>
+  <si>
+    <t>Pegasys</t>
+  </si>
+  <si>
+    <t>US-EIN-042103594-GCCI-3978870</t>
+  </si>
+  <si>
+    <t>J-PAL</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300049</t>
   </si>
 </sst>
 </file>
@@ -642,11 +669,11 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1117,6 +1144,57 @@
       </c>
       <c r="E28" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1153,6 +1231,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6713CC7F31D7C498DF06765AF1263E4" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="49295815813be5682bd1502ac40ad112">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="9e449739-2858-4f41-8e5c-7dc6df20853e" xmlns:ns4="05c15269-663a-4da2-bb2b-1510839404b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57db594e689bb932d2839527134c19ea" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1386,15 +1473,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
   <ds:schemaRefs>
@@ -1406,6 +1484,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E21D5880-A9EF-4322-906E-79CE5A8FFAC1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1423,12 +1509,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Script 0 (set up) created
Functions, package installation, input data and reference lookups moved to standalone script for better maintenance
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dfid-my.sharepoint.com/personal/e-clegg_dfid_gov_uk/Documents/Github Projects/ODA_research_and_innovation/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{1F8182CB-FE63-4525-B953-FF5A791C5CBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{154CDFCA-834D-4DD5-94FD-EE2B301E65AB}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{1F8182CB-FE63-4525-B953-FF5A791C5CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{154CDFCA-834D-4DD5-94FD-EE2B301E65AB}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="420" windowWidth="25440" windowHeight="15390" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
   <sheets>
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
@@ -672,20 +672,20 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.75" customWidth="1"/>
-    <col min="2" max="2" width="42.08203125" customWidth="1"/>
-    <col min="3" max="3" width="31.75" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="37.25" customWidth="1"/>
+    <col min="1" max="1" width="54.69921875" customWidth="1"/>
+    <col min="2" max="2" width="42.09765625" customWidth="1"/>
+    <col min="3" max="3" width="31.69921875" customWidth="1"/>
+    <col min="4" max="4" width="30.296875" customWidth="1"/>
+    <col min="5" max="5" width="37.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,7 +702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -719,7 +719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -736,7 +736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -753,7 +753,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -770,7 +770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -787,7 +787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -804,7 +804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -821,7 +821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -838,7 +838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -852,7 +852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -866,7 +866,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -883,7 +883,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -897,7 +897,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -911,7 +911,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -925,7 +925,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -942,7 +942,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -959,7 +959,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -976,7 +976,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -993,7 +993,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -1222,21 +1222,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1474,19 +1474,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
IATI partner org extract simplified
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clegge\OneDrive - Wellcome Cloud\My Documents\GitHub\ODA_research_and_innovation\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{1F8182CB-FE63-4525-B953-FF5A791C5CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{807FF33F-E8C9-4833-BB52-4319932C3426}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A5F7B8-FFA1-4BEE-80A4-3423072EAED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
   <sheets>
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
   <si>
     <t>iati_id</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>FCDO Research - Programmes</t>
+  </si>
+  <si>
+    <t>GB-COH-877338-GV-GOV-1-300708-124</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300708-124</t>
   </si>
 </sst>
 </file>
@@ -624,7 +630,7 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1006,6 +1012,23 @@
       </c>
       <c r="E22" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1033,21 +1056,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1285,19 +1308,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tableau country unknowns limited
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clegge\OneDrive - Wellcome Cloud\My Documents\GitHub\ODA_research_and_innovation\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A5F7B8-FFA1-4BEE-80A4-3423072EAED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E9A5F7B8-FFA1-4BEE-80A4-3423072EAED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{64F0F95E-56EE-4481-852C-6805DE309CA9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$889</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$888</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
   <si>
     <t>iati_id</t>
   </si>
@@ -93,15 +93,6 @@
   </si>
   <si>
     <t>ZA-NPO-048-364-FCFA_AG_Programme</t>
-  </si>
-  <si>
-    <t>CA-CRA_ACR-811793611-HGC</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300574</t>
-  </si>
-  <si>
-    <t>Grand Challenges Canada</t>
   </si>
   <si>
     <t>GB-EDU-133784-TWPCOP</t>
@@ -630,11 +621,11 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -674,7 +665,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -691,7 +682,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -708,7 +699,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -725,7 +716,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -742,7 +733,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -759,7 +750,7 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -772,39 +763,39 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
         <v>27</v>
@@ -821,7 +812,7 @@
         <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -838,7 +829,7 @@
         <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
@@ -846,53 +837,53 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
         <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -906,7 +897,7 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
         <v>43</v>
@@ -923,44 +914,44 @@
         <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
         <v>47</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
-      </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
         <v>50</v>
-      </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,7 +965,7 @@
         <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>
@@ -988,18 +979,18 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
         <v>55</v>
-      </c>
-      <c r="D21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -1008,33 +999,16 @@
         <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E889" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E49">
-      <sortCondition ref="A1:A889"/>
+  <autoFilter ref="A1:E888" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E48">
+      <sortCondition ref="A1:A888"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1056,21 +1030,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1308,19 +1282,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
UKRI research council names changed
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E9A5F7B8-FFA1-4BEE-80A4-3423072EAED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00D1B42A-AF02-47E8-BCBF-7AD07737BDBE}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{E9A5F7B8-FFA1-4BEE-80A4-3423072EAED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8869EA8-43CC-4EC4-88B4-129F346B316B}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
   <sheets>
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$886</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$884</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>iati_id</t>
   </si>
@@ -116,15 +116,6 @@
     <t>Acumen</t>
   </si>
   <si>
-    <t>IN-MCA-U74140DL1998PLC097579-1662_AGRITECH-CATALYST_DFID_UK</t>
-  </si>
-  <si>
-    <t>GB-1-203067</t>
-  </si>
-  <si>
-    <t>IPE Global</t>
-  </si>
-  <si>
     <t>GB-COH-877338-RF15005</t>
   </si>
   <si>
@@ -185,15 +176,6 @@
     <t>Pegasys</t>
   </si>
   <si>
-    <t>US-EIN-042103594-GCCI-3978870</t>
-  </si>
-  <si>
-    <t>J-PAL</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300049</t>
-  </si>
-  <si>
     <t>FCDO Research - Programmes</t>
   </si>
   <si>
@@ -201,6 +183,15 @@
   </si>
   <si>
     <t>GB-GOV-1-300708-124</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300397</t>
+  </si>
+  <si>
+    <t>LSHTM</t>
+  </si>
+  <si>
+    <t>GB-EDU-133903-PENDA</t>
   </si>
 </sst>
 </file>
@@ -606,11 +597,11 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -650,7 +641,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -667,7 +658,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -684,7 +675,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -701,7 +692,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -718,7 +709,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -735,7 +726,7 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -766,7 +757,7 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
@@ -783,7 +774,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
@@ -791,53 +782,53 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -851,44 +842,44 @@
         <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
         <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -902,7 +893,7 @@
         <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
         <v>45</v>
@@ -910,59 +901,42 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>51</v>
-      </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E886" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E46">
-      <sortCondition ref="A1:A886"/>
+  <autoFilter ref="A1:E884" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E44">
+      <sortCondition ref="A1:A884"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Script 1 and 2 tidied/commented
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e-clegg\Documents\GitHub projects\ODA_research_and_innovation\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{E9A5F7B8-FFA1-4BEE-80A4-3423072EAED5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8869EA8-43CC-4EC4-88B4-129F346B316B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D131B8AF-0BE9-48A5-B77E-60C230EFD56A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
   <sheets>
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$884</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$885</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
   <si>
     <t>iati_id</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>GB-EDU-133903-PENDA</t>
+  </si>
+  <si>
+    <t>US-EIN-134166228-GB-GOV-1-300123-101-ACUMEN-MECS</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300123</t>
   </si>
 </sst>
 </file>
@@ -597,23 +603,23 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.69921875" customWidth="1"/>
-    <col min="2" max="2" width="42.09765625" customWidth="1"/>
-    <col min="3" max="3" width="31.69921875" customWidth="1"/>
-    <col min="4" max="4" width="30.296875" customWidth="1"/>
-    <col min="5" max="5" width="37.19921875" customWidth="1"/>
+    <col min="1" max="1" width="54.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.08203125" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="37.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -647,7 +653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -664,7 +670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -681,7 +687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -698,7 +704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -715,7 +721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -732,7 +738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -746,7 +752,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -763,180 +769,197 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
         <v>41</v>
       </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>47</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
         <v>48</v>
       </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
         <v>49</v>
       </c>
-      <c r="D19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E884" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E44">
-      <sortCondition ref="A1:A884"/>
+  <autoFilter ref="A1:E885" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E45">
+      <sortCondition ref="A1:A885"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -958,24 +981,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6713CC7F31D7C498DF06765AF1263E4" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="49295815813be5682bd1502ac40ad112">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="9e449739-2858-4f41-8e5c-7dc6df20853e" xmlns:ns4="05c15269-663a-4da2-bb2b-1510839404b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57db594e689bb932d2839527134c19ea" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1209,25 +1214,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E21D5880-A9EF-4322-906E-79CE5A8FFAC1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1245,4 +1250,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Missing iati.cloud activities troubleshooted
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e-clegg\Documents\GitHub projects\ODA_research_and_innovation\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D131B8AF-0BE9-48A5-B77E-60C230EFD56A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D131B8AF-0BE9-48A5-B77E-60C230EFD56A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAB7C458-0BE9-41B3-8A00-222C4A3D702E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
   <sheets>
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t>iati_id</t>
   </si>
@@ -198,13 +198,28 @@
   </si>
   <si>
     <t>GB-GOV-1-300123</t>
+  </si>
+  <si>
+    <t>US-EIN-042103594-GCCI-3978870</t>
+  </si>
+  <si>
+    <t>GB-GOV-1-300049</t>
+  </si>
+  <si>
+    <t>J-PAL</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>not being returned as a linked activity in iati.cloud extraction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +235,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -250,11 +271,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,23 +625,24 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" customWidth="1"/>
-    <col min="2" max="2" width="42.08203125" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="37.1640625" customWidth="1"/>
+    <col min="1" max="1" width="54.69921875" customWidth="1"/>
+    <col min="2" max="2" width="42.09765625" customWidth="1"/>
+    <col min="3" max="3" width="31.69921875" customWidth="1"/>
+    <col min="4" max="4" width="30.296875" customWidth="1"/>
+    <col min="5" max="5" width="37.19921875" customWidth="1"/>
+    <col min="6" max="6" width="40.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,8 +658,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -653,7 +679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -670,7 +696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -687,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -704,7 +730,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -721,7 +747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -738,7 +764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -752,7 +778,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -769,7 +795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -786,7 +812,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -803,7 +829,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -820,7 +846,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -837,7 +863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -854,7 +880,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -871,7 +897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -888,7 +914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -905,7 +931,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -922,7 +948,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -939,7 +965,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -954,6 +980,26 @@
       </c>
       <c r="E20" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -981,6 +1027,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6713CC7F31D7C498DF06765AF1263E4" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="49295815813be5682bd1502ac40ad112">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="9e449739-2858-4f41-8e5c-7dc6df20853e" xmlns:ns4="05c15269-663a-4da2-bb2b-1510839404b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57db594e689bb932d2839527134c19ea" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1214,15 +1269,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1233,6 +1279,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E21D5880-A9EF-4322-906E-79CE5A8FFAC1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1252,14 +1306,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Transactions extraction updated (to include orgs)
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D131B8AF-0BE9-48A5-B77E-60C230EFD56A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAB7C458-0BE9-41B3-8A00-222C4A3D702E}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{D131B8AF-0BE9-48A5-B77E-60C230EFD56A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{B751C9A5-7083-4CCB-A3D2-B26337629885}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$885</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$876</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>iati_id</t>
   </si>
@@ -59,24 +59,12 @@
     <t>British Council</t>
   </si>
   <si>
-    <t>GB-COH-05543952-GB-1-203048</t>
-  </si>
-  <si>
-    <t>GB-1-203048</t>
-  </si>
-  <si>
-    <t>Cardno Emerging Markets</t>
-  </si>
-  <si>
     <t>GB-1-204867</t>
   </si>
   <si>
     <t>University of Manchester</t>
   </si>
   <si>
-    <t>ZA-NPO-048-364-FCFA_AG_CCKE</t>
-  </si>
-  <si>
     <t>GB-1-203835</t>
   </si>
   <si>
@@ -86,15 +74,6 @@
     <t>ZA-NPO-048-364-FCFA_AG_ADAPTATIONRESEARCHALLIANCE</t>
   </si>
   <si>
-    <t>ZA-NPO-048-364-FCFA_AG_ClimateMainstreamingFacility</t>
-  </si>
-  <si>
-    <t>ZA-NPO-048-364-FCFA_AG_ModelEvaluationHub/LaunchPad</t>
-  </si>
-  <si>
-    <t>ZA-NPO-048-364-FCFA_AG_Programme</t>
-  </si>
-  <si>
     <t>GB-COH-RC000660-WAR-PATH</t>
   </si>
   <si>
@@ -167,59 +146,23 @@
     <t>Results for Development</t>
   </si>
   <si>
-    <t>GB-COH-10333897-(SMEP) PROGRAMME – PROGRAMME MANAGEMENT COMPONENT</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300124</t>
-  </si>
-  <si>
-    <t>Pegasys</t>
-  </si>
-  <si>
     <t>FCDO Research - Programmes</t>
   </si>
   <si>
-    <t>GB-COH-877338-GV-GOV-1-300708-124</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300708-124</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300397</t>
-  </si>
-  <si>
-    <t>LSHTM</t>
-  </si>
-  <si>
-    <t>GB-EDU-133903-PENDA</t>
-  </si>
-  <si>
     <t>US-EIN-134166228-GB-GOV-1-300123-101-ACUMEN-MECS</t>
   </si>
   <si>
     <t>GB-GOV-1-300123</t>
   </si>
   <si>
-    <t>US-EIN-042103594-GCCI-3978870</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300049</t>
-  </si>
-  <si>
-    <t>J-PAL</t>
-  </si>
-  <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>not being returned as a linked activity in iati.cloud extraction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,12 +178,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -271,27 +208,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -625,11 +551,11 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -659,24 +585,24 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -684,95 +610,95 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -780,243 +706,84 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" t="s">
-        <v>58</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E885" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E45">
-      <sortCondition ref="A1:A885"/>
+  <autoFilter ref="A1:E876" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
+      <sortCondition ref="A1:A876"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5 A1:A3 A7:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  <conditionalFormatting sqref="A3:A1048576 A1">
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Q3 2021-22 data update
</commit_message>
<xml_diff>
--- a/Inputs/IATI partner activities.xlsx
+++ b/Inputs/IATI partner activities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{D131B8AF-0BE9-48A5-B77E-60C230EFD56A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{B751C9A5-7083-4CCB-A3D2-B26337629885}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{D131B8AF-0BE9-48A5-B77E-60C230EFD56A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAA942E2-0EB9-4AF3-9AF1-C85C2337EE17}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF2F4B21-F468-4F3D-9B32-1F43EB9441E3}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IATI activity IDs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$876</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IATI activity IDs'!$A$1:$E$870</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
-  <si>
-    <t>iati_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>gov_funder</t>
   </si>
   <si>
-    <t>funding_iati_id</t>
-  </si>
-  <si>
     <t>fund</t>
   </si>
   <si>
@@ -59,42 +53,9 @@
     <t>British Council</t>
   </si>
   <si>
-    <t>GB-1-204867</t>
-  </si>
-  <si>
     <t>University of Manchester</t>
   </si>
   <si>
-    <t>GB-1-203835</t>
-  </si>
-  <si>
-    <t>SouthSouthNorth</t>
-  </si>
-  <si>
-    <t>ZA-NPO-048-364-FCFA_AG_ADAPTATIONRESEARCHALLIANCE</t>
-  </si>
-  <si>
-    <t>GB-COH-RC000660-WAR-PATH</t>
-  </si>
-  <si>
-    <t>Department of Health and Social Care</t>
-  </si>
-  <si>
-    <t>Global Health Research - Programmes</t>
-  </si>
-  <si>
-    <t>University of Liverpool</t>
-  </si>
-  <si>
-    <t>US-EIN-134166228-GB-GOV-1-300632-102</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300632</t>
-  </si>
-  <si>
-    <t>Acumen</t>
-  </si>
-  <si>
     <t>GB-COH-877338-RF15005</t>
   </si>
   <si>
@@ -113,18 +74,6 @@
     <t>GB-1-203051</t>
   </si>
   <si>
-    <t>US-EIN-134166228-GB-COH-06274284-TEA2 - PIONEER ENERGY INVESTMENT INITIATIVE 2</t>
-  </si>
-  <si>
-    <t>US-EIN-91-1157127-RHSC_PROGRAM_2020-2025_(300713-103)</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300341</t>
-  </si>
-  <si>
-    <t>PATH</t>
-  </si>
-  <si>
     <t>GB-COH-RC000797-GB-GOV-1-300180</t>
   </si>
   <si>
@@ -149,13 +98,10 @@
     <t>FCDO Research - Programmes</t>
   </si>
   <si>
-    <t>US-EIN-134166228-GB-GOV-1-300123-101-ACUMEN-MECS</t>
-  </si>
-  <si>
-    <t>GB-GOV-1-300123</t>
-  </si>
-  <si>
-    <t>Notes</t>
+    <t>iati_identifier</t>
+  </si>
+  <si>
+    <t>activity_id</t>
   </si>
 </sst>
 </file>
@@ -217,17 +163,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -551,11 +487,11 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -565,224 +501,118 @@
     <col min="3" max="3" width="31.69921875" customWidth="1"/>
     <col min="4" max="4" width="30.296875" customWidth="1"/>
     <col min="5" max="5" width="37.19921875" customWidth="1"/>
-    <col min="6" max="6" width="40.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E876" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
-      <sortCondition ref="A1:A876"/>
+  <autoFilter ref="A1:E870" xr:uid="{6E007EFC-ECCE-421D-B554-61739E668986}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E30">
+      <sortCondition ref="A1:A870"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A1048576 A1">
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -794,15 +624,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6713CC7F31D7C498DF06765AF1263E4" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="49295815813be5682bd1502ac40ad112">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="9e449739-2858-4f41-8e5c-7dc6df20853e" xmlns:ns4="05c15269-663a-4da2-bb2b-1510839404b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57db594e689bb932d2839527134c19ea" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1036,6 +857,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1046,14 +876,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E21D5880-A9EF-4322-906E-79CE5A8FFAC1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1073,6 +895,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4115639F-0FB6-4C25-A530-2B8A26AA3E24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{145BBD6B-A846-4263-BED8-B399B91A0B7C}">
   <ds:schemaRefs>

</xml_diff>